<commit_message>
ADDED: notif channel entity
</commit_message>
<xml_diff>
--- a/templates/sample.xlsx
+++ b/templates/sample.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,24 +425,27 @@
         <v>Release Date</v>
       </c>
       <c r="H1" t="str">
+        <v>Thumbnail URL</v>
+      </c>
+      <c r="I1" t="str">
         <v>Shelf-A</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Shelf-B</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>Shelf-C</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>Shelf-D</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>Shelf-E</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>